<commit_message>
Adding of Transaction Form and List
</commit_message>
<xml_diff>
--- a/Documents/Accountint Excel Files/الجانب الدائن/قطف.xlsx
+++ b/Documents/Accountint Excel Files/الجانب الدائن/قطف.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="15600" windowHeight="11760"/>
@@ -11,7 +11,7 @@
     <sheet name="ورقة2" sheetId="2" r:id="rId2"/>
     <sheet name="ورقة3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -54,15 +54,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -71,7 +71,7 @@
       <b/>
       <sz val="26"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -79,14 +79,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="26"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -95,7 +95,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -229,45 +229,6 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -282,6 +243,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -290,11 +290,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="سمة Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -368,6 +373,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -402,6 +408,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -577,705 +584,705 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="16">
         <f>F30-G30</f>
         <v>0</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" ht="18">
-      <c r="A4" s="14" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18">
-      <c r="A5" s="15">
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="3">
         <v>43808</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D5" s="15">
-        <v>290</v>
-      </c>
-      <c r="E5" s="15">
+      <c r="D5" s="2">
+        <v>290</v>
+      </c>
+      <c r="E5" s="2">
         <f>C5*D5</f>
         <v>1479</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="2">
         <f>E5</f>
         <v>1479</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="2">
         <v>8000</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="3">
         <v>43811</v>
       </c>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" ht="18">
-      <c r="A6" s="15">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="4">
         <v>5.3120000000000003</v>
       </c>
-      <c r="D6" s="15">
-        <v>290</v>
-      </c>
-      <c r="E6" s="15">
+      <c r="D6" s="2">
+        <v>290</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" ref="E6:E29" si="0">C6*D6</f>
         <v>1540.48</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="2">
         <f>E6+F5</f>
         <v>3019.48</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="2">
         <v>7000</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="3">
         <v>43819</v>
       </c>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" ht="18">
-      <c r="A7" s="15">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="4">
         <v>5.242</v>
       </c>
-      <c r="D7" s="15">
-        <v>290</v>
-      </c>
-      <c r="E7" s="15">
+      <c r="D7" s="2">
+        <v>290</v>
+      </c>
+      <c r="E7" s="2">
         <f>C7*D7</f>
         <v>1520.18</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="2">
         <f t="shared" ref="F7:F30" si="1">E7+F6</f>
         <v>4539.66</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="2">
         <v>100</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="3">
         <v>43822</v>
       </c>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9" ht="18">
-      <c r="A8" s="15">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="3">
         <v>43809</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="4">
         <v>5.5650000000000004</v>
       </c>
-      <c r="D8" s="15">
-        <v>290</v>
-      </c>
-      <c r="E8" s="15">
+      <c r="D8" s="2">
+        <v>290</v>
+      </c>
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>1613.8500000000001</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>6153.51</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="2">
         <v>2500</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="3">
         <v>43824</v>
       </c>
-      <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="1:9" ht="18">
-      <c r="A9" s="15">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="4">
         <v>5.27</v>
       </c>
-      <c r="D9" s="15">
-        <v>290</v>
-      </c>
-      <c r="E9" s="15">
+      <c r="D9" s="2">
+        <v>290</v>
+      </c>
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>1528.3</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>7681.81</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="2">
         <v>4404</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:9" ht="18">
-      <c r="A10" s="15">
+      <c r="H9" s="3"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="4">
         <v>5.47</v>
       </c>
-      <c r="D10" s="15">
-        <v>290</v>
-      </c>
-      <c r="E10" s="15">
+      <c r="D10" s="2">
+        <v>290</v>
+      </c>
+      <c r="E10" s="2">
         <f>C10*D10</f>
         <v>1586.3</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>9268.11</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="2">
         <v>0.51</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" ht="18">
-      <c r="A11" s="15">
+      <c r="H10" s="3"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>7</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="3">
         <v>43810</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="4">
         <v>5.2549999999999999</v>
       </c>
-      <c r="D11" s="15">
-        <v>290</v>
-      </c>
-      <c r="E11" s="15">
+      <c r="D11" s="2">
+        <v>290</v>
+      </c>
+      <c r="E11" s="2">
         <f>C11*D11</f>
         <v>1523.95</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>10792.060000000001</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="18"/>
-    </row>
-    <row r="12" spans="1:9" ht="18">
-      <c r="A12" s="15">
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="4">
         <v>5.2</v>
       </c>
-      <c r="D12" s="15">
-        <v>290</v>
-      </c>
-      <c r="E12" s="15">
+      <c r="D12" s="2">
+        <v>290</v>
+      </c>
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>1508</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
         <v>12300.060000000001</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="18"/>
-    </row>
-    <row r="13" spans="1:9" ht="18">
-      <c r="A13" s="15">
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="4">
         <v>4.9249999999999998</v>
       </c>
-      <c r="D13" s="15">
-        <v>290</v>
-      </c>
-      <c r="E13" s="15">
+      <c r="D13" s="2">
+        <v>290</v>
+      </c>
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>1428.25</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>13728.310000000001</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" spans="1:9" ht="18">
-      <c r="A14" s="15">
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>10</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="3">
         <v>43811</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="4">
         <v>3700</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>3700</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>17428.310000000001</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="18"/>
-    </row>
-    <row r="15" spans="1:9" ht="18">
-      <c r="A15" s="15">
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="3">
         <v>43813</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="4">
         <v>5.4550000000000001</v>
       </c>
-      <c r="D15" s="15">
-        <v>290</v>
-      </c>
-      <c r="E15" s="15">
+      <c r="D15" s="2">
+        <v>290</v>
+      </c>
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>1581.95</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="2">
         <f t="shared" si="1"/>
         <v>19010.260000000002</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="18"/>
-    </row>
-    <row r="16" spans="1:9" ht="18">
-      <c r="A16" s="15">
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="4">
         <v>5.36</v>
       </c>
-      <c r="D16" s="15">
-        <v>290</v>
-      </c>
-      <c r="E16" s="15">
+      <c r="D16" s="2">
+        <v>290</v>
+      </c>
+      <c r="E16" s="2">
         <f t="shared" si="0"/>
         <v>1554.4</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="2">
         <f t="shared" si="1"/>
         <v>20564.660000000003</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="18"/>
-    </row>
-    <row r="17" spans="1:9" ht="18">
-      <c r="A17" s="15">
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>13</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="4">
         <v>4.9649999999999999</v>
       </c>
-      <c r="D17" s="15">
-        <v>290</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="D17" s="2">
+        <v>290</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="0"/>
         <v>1439.85</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="18"/>
-    </row>
-    <row r="18" spans="1:9" ht="18">
-      <c r="A18" s="15">
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="15">
-        <v>290</v>
-      </c>
-      <c r="E18" s="15">
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="2">
+        <v>290</v>
+      </c>
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="18"/>
-    </row>
-    <row r="19" spans="1:9" ht="18" hidden="1">
-      <c r="A19" s="15">
+      <c r="G18" s="2"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>15</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="15">
-        <v>290</v>
-      </c>
-      <c r="E19" s="15">
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="2">
+        <v>290</v>
+      </c>
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="18"/>
-    </row>
-    <row r="20" spans="1:9" ht="18" hidden="1">
-      <c r="A20" s="15">
+      <c r="G19" s="2"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>16</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="15">
-        <v>290</v>
-      </c>
-      <c r="E20" s="15">
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2">
+        <v>290</v>
+      </c>
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="18"/>
-    </row>
-    <row r="21" spans="1:9" ht="18" hidden="1">
-      <c r="A21" s="15">
+      <c r="G20" s="2"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>17</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="15">
-        <v>290</v>
-      </c>
-      <c r="E21" s="15">
+      <c r="B21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="2">
+        <v>290</v>
+      </c>
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="18"/>
-    </row>
-    <row r="22" spans="1:9" ht="18" hidden="1">
-      <c r="A22" s="15">
+      <c r="G21" s="2"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>18</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="15">
-        <v>290</v>
-      </c>
-      <c r="E22" s="15">
+      <c r="B22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="2">
+        <v>290</v>
+      </c>
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="18"/>
-    </row>
-    <row r="23" spans="1:9" ht="18" hidden="1">
-      <c r="A23" s="15">
+      <c r="G22" s="2"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>19</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="15">
-        <v>290</v>
-      </c>
-      <c r="E23" s="15">
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="2">
+        <v>290</v>
+      </c>
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="18"/>
-    </row>
-    <row r="24" spans="1:9" ht="18" hidden="1">
-      <c r="A24" s="15">
+      <c r="G23" s="2"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>20</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="15">
-        <v>290</v>
-      </c>
-      <c r="E24" s="15">
+      <c r="B24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="2">
+        <v>290</v>
+      </c>
+      <c r="E24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="18"/>
-    </row>
-    <row r="25" spans="1:9" ht="18" hidden="1">
-      <c r="A25" s="15">
+      <c r="G24" s="2"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>21</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="15">
-        <v>290</v>
-      </c>
-      <c r="E25" s="15">
+      <c r="B25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="2">
+        <v>290</v>
+      </c>
+      <c r="E25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:9" ht="18" hidden="1">
-      <c r="A26" s="15">
+      <c r="G25" s="2"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="15">
-        <v>290</v>
-      </c>
-      <c r="E26" s="15">
+      <c r="B26" s="2"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="2">
+        <v>290</v>
+      </c>
+      <c r="E26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="18"/>
-    </row>
-    <row r="27" spans="1:9" ht="18" hidden="1">
-      <c r="A27" s="15">
+      <c r="G26" s="2"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="15">
-        <v>290</v>
-      </c>
-      <c r="E27" s="15">
+      <c r="B27" s="2"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="2">
+        <v>290</v>
+      </c>
+      <c r="E27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="1:9" ht="18" hidden="1">
-      <c r="A28" s="15">
+      <c r="G27" s="2"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>24</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="15">
-        <v>290</v>
-      </c>
-      <c r="E28" s="15">
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="2">
+        <v>290</v>
+      </c>
+      <c r="E28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="18"/>
-    </row>
-    <row r="29" spans="1:9" ht="18" hidden="1">
-      <c r="A29" s="15">
+      <c r="G28" s="2"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>25</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="15">
-        <v>290</v>
-      </c>
-      <c r="E29" s="15">
+      <c r="B29" s="2"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="2">
+        <v>290</v>
+      </c>
+      <c r="E29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="18"/>
-    </row>
-    <row r="30" spans="1:9" ht="18">
-      <c r="A30" s="14" t="s">
+      <c r="G29" s="2"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2">
         <f t="shared" si="1"/>
         <v>22004.510000000002</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="1">
         <f>SUM(G5:G29)</f>
         <v>22004.51</v>
       </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1288,12 +1295,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1301,12 +1308,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>